<commit_message>
Stedelijk, randstedelijk,... vertaald naar Engelse
</commit_message>
<xml_diff>
--- a/Asian hornet data.xlsx
+++ b/Asian hornet data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\helee\OneDrive\Documenten\GitHub\vespa_analyses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc989a75547cfb81/Documenten/GitHub/vespa_analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDA70BF-EF32-441A-AF65-BAFDBD15F301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{2FDA70BF-EF32-441A-AF65-BAFDBD15F301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{683ACDBA-9D53-439F-B911-B59D1D84CC0A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D21F6F35-0DF4-4740-B8AA-5A49382E1DF7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="8" xr2:uid="{D21F6F35-0DF4-4740-B8AA-5A49382E1DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Flights" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4020" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4021" uniqueCount="261">
   <si>
     <t>Date</t>
   </si>
@@ -829,6 +829,9 @@
   <si>
     <t>Verstedelijkt</t>
   </si>
+  <si>
+    <t>Urban_EN</t>
+  </si>
 </sst>
 </file>
 
@@ -1290,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88DC3462-51EA-49F0-8541-5518B67248DA}">
   <dimension ref="A1:V285"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="92" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A197" sqref="A197:XFD197"/>
     </sheetView>
   </sheetViews>
@@ -29118,7 +29121,7 @@
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
-        <f t="shared" ref="A65:A97" si="9">A64+1</f>
+        <f t="shared" ref="A65:A95" si="9">A64+1</f>
         <v>64</v>
       </c>
       <c r="B65" s="31">
@@ -58489,7 +58492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25DE0E8-20D7-42E5-A5FE-9568E58C2604}">
   <dimension ref="A1:N157"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H1:H2"/>
     </sheetView>
@@ -62127,11 +62130,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FFDA88-3512-4357-B275-C59183D0EF18}">
-  <dimension ref="A1:N89"/>
+  <dimension ref="A1:O89"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" zoomScale="121" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N90" sqref="N90"/>
+    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -62144,9 +62147,10 @@
     <col min="8" max="8" width="15.77734375" customWidth="1"/>
     <col min="9" max="9" width="16.44140625" customWidth="1"/>
     <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="15" max="15" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -62189,8 +62193,11 @@
       <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -62234,8 +62241,12 @@
       <c r="N2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2" t="str">
+        <f>IF(N2="Landelijk", "Rural", IF(N2="Randstedelijk", "Suburban", "Urban"))</f>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -62279,8 +62290,12 @@
       <c r="N3" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O66" si="1">IF(N3="Landelijk", "Rural", IF(N3="Randstedelijk", "Suburban", "Urban"))</f>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -62324,8 +62339,12 @@
       <c r="N4" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -62369,8 +62388,12 @@
       <c r="N5" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O5" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -62414,8 +62437,12 @@
       <c r="N6" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O6" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10</v>
       </c>
@@ -62432,7 +62459,7 @@
         <v>332</v>
       </c>
       <c r="F7" s="7">
-        <f t="shared" ref="F7:F57" si="1">MOD(180+G7,360)</f>
+        <f t="shared" ref="F7:F57" si="2">MOD(180+G7,360)</f>
         <v>83.899999999999977</v>
       </c>
       <c r="G7" s="7">
@@ -62459,8 +62486,12 @@
       <c r="N7" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O7" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10</v>
       </c>
@@ -62477,7 +62508,7 @@
         <v>301</v>
       </c>
       <c r="F8" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>64.899999999999977</v>
       </c>
       <c r="G8" s="7">
@@ -62504,8 +62535,12 @@
       <c r="N8" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O8" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10</v>
       </c>
@@ -62522,7 +62557,7 @@
         <v>203</v>
       </c>
       <c r="F9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="G9" s="7">
@@ -62549,8 +62584,12 @@
       <c r="N9" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O9" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -62567,7 +62606,7 @@
         <v>274</v>
       </c>
       <c r="F10" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="G10" s="7">
@@ -62594,8 +62633,12 @@
       <c r="N10" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O10" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -62612,7 +62655,7 @@
         <v>196</v>
       </c>
       <c r="F11" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="G11" s="7">
@@ -62639,8 +62682,12 @@
       <c r="N11" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O11" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -62657,7 +62704,7 @@
         <v>184</v>
       </c>
       <c r="F12" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="G12" s="7">
@@ -62684,8 +62731,12 @@
       <c r="N12" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O12" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
@@ -62702,7 +62753,7 @@
         <v>141</v>
       </c>
       <c r="F13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="G13" s="7">
@@ -62729,8 +62780,12 @@
       <c r="N13" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O13" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10</v>
       </c>
@@ -62747,7 +62802,7 @@
         <v>54</v>
       </c>
       <c r="F14" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>338</v>
       </c>
       <c r="G14" s="7">
@@ -62774,8 +62829,12 @@
       <c r="N14" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O14" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>11</v>
       </c>
@@ -62792,7 +62851,7 @@
         <v>746</v>
       </c>
       <c r="F15" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>135.5</v>
       </c>
       <c r="G15" s="7">
@@ -62819,8 +62878,12 @@
       <c r="N15" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O15" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>12</v>
       </c>
@@ -62837,7 +62900,7 @@
         <v>134</v>
       </c>
       <c r="F16" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>238</v>
       </c>
       <c r="G16" s="7">
@@ -62864,8 +62927,12 @@
       <c r="N16" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O16" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>13</v>
       </c>
@@ -62882,7 +62949,7 @@
         <v>652</v>
       </c>
       <c r="F17" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>169</v>
       </c>
       <c r="G17" s="7">
@@ -62909,8 +62976,12 @@
       <c r="N17" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O17" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>13</v>
       </c>
@@ -62927,7 +62998,7 @@
         <v>415</v>
       </c>
       <c r="F18" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>307.10000000000002</v>
       </c>
       <c r="G18" s="7">
@@ -62954,8 +63025,12 @@
       <c r="N18" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O18" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>13</v>
       </c>
@@ -62972,7 +63047,7 @@
         <v>401</v>
       </c>
       <c r="F19" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65.699999999999989</v>
       </c>
       <c r="G19" s="7">
@@ -62999,8 +63074,12 @@
       <c r="N19" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O19" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>14</v>
       </c>
@@ -63017,7 +63096,7 @@
         <v>157</v>
       </c>
       <c r="F20" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>173</v>
       </c>
       <c r="G20" s="7">
@@ -63044,8 +63123,12 @@
       <c r="N20" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O20" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>14</v>
       </c>
@@ -63062,7 +63145,7 @@
         <v>270</v>
       </c>
       <c r="F21" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G21" s="7">
@@ -63089,8 +63172,12 @@
       <c r="N21" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O21" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>14</v>
       </c>
@@ -63107,7 +63194,7 @@
         <v>232</v>
       </c>
       <c r="F22" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>268</v>
       </c>
       <c r="G22" s="7">
@@ -63134,8 +63221,12 @@
       <c r="N22" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O22" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>14</v>
       </c>
@@ -63152,7 +63243,7 @@
         <v>413</v>
       </c>
       <c r="F23" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>219.9</v>
       </c>
       <c r="G23" s="7">
@@ -63179,8 +63270,12 @@
       <c r="N23" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O23" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>15</v>
       </c>
@@ -63197,7 +63292,7 @@
         <v>313</v>
       </c>
       <c r="F24" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>241.1</v>
       </c>
       <c r="G24" s="7">
@@ -63224,8 +63319,12 @@
       <c r="N24" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O24" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>16</v>
       </c>
@@ -63242,7 +63341,7 @@
         <v>139</v>
       </c>
       <c r="F25" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>252</v>
       </c>
       <c r="G25" s="7">
@@ -63269,8 +63368,12 @@
       <c r="N25" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O25" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>16</v>
       </c>
@@ -63287,7 +63390,7 @@
         <v>70</v>
       </c>
       <c r="F26" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>277</v>
       </c>
       <c r="G26" s="7">
@@ -63314,8 +63417,12 @@
       <c r="N26" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O26" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>16</v>
       </c>
@@ -63332,7 +63439,7 @@
         <v>92</v>
       </c>
       <c r="F27" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>217</v>
       </c>
       <c r="G27" s="7">
@@ -63359,8 +63466,12 @@
       <c r="N27" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O27" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>16</v>
       </c>
@@ -63377,7 +63488,7 @@
         <v>181</v>
       </c>
       <c r="F28" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>223</v>
       </c>
       <c r="G28" s="7">
@@ -63404,8 +63515,12 @@
       <c r="N28" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O28" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>16</v>
       </c>
@@ -63422,7 +63537,7 @@
         <v>84</v>
       </c>
       <c r="F29" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>242</v>
       </c>
       <c r="G29" s="7">
@@ -63449,8 +63564,12 @@
       <c r="N29" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O29" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>16</v>
       </c>
@@ -63467,7 +63586,7 @@
         <v>83</v>
       </c>
       <c r="F30" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="G30" s="7">
@@ -63494,8 +63613,12 @@
       <c r="N30" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O30" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>17</v>
       </c>
@@ -63512,7 +63635,7 @@
         <v>415</v>
       </c>
       <c r="F31" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>119.39999999999998</v>
       </c>
       <c r="G31" s="7">
@@ -63539,8 +63662,12 @@
       <c r="N31" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O31" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>17</v>
       </c>
@@ -63557,7 +63684,7 @@
         <v>187</v>
       </c>
       <c r="F32" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>130</v>
       </c>
       <c r="G32" s="7">
@@ -63584,8 +63711,12 @@
       <c r="N32" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O32" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>18</v>
       </c>
@@ -63602,7 +63733,7 @@
         <v>706</v>
       </c>
       <c r="F33" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>240.8</v>
       </c>
       <c r="G33" s="7">
@@ -63629,8 +63760,12 @@
       <c r="N33" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O33" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>18</v>
       </c>
@@ -63647,7 +63782,7 @@
         <v>331</v>
       </c>
       <c r="F34" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>251.6</v>
       </c>
       <c r="G34" s="7">
@@ -63674,8 +63809,12 @@
       <c r="N34" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O34" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>18</v>
       </c>
@@ -63692,7 +63831,7 @@
         <v>230</v>
       </c>
       <c r="F35" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244</v>
       </c>
       <c r="G35" s="7">
@@ -63719,8 +63858,12 @@
       <c r="N35" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O35" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>18</v>
       </c>
@@ -63737,7 +63880,7 @@
         <v>110</v>
       </c>
       <c r="F36" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>102</v>
       </c>
       <c r="G36" s="7">
@@ -63764,8 +63907,12 @@
       <c r="N36" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O36" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>19</v>
       </c>
@@ -63782,7 +63929,7 @@
         <v>340</v>
       </c>
       <c r="F37" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>83.800000000000011</v>
       </c>
       <c r="G37" s="7">
@@ -63809,8 +63956,12 @@
       <c r="N37" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O37" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>20</v>
       </c>
@@ -63827,7 +63978,7 @@
         <v>188</v>
       </c>
       <c r="F38" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>313</v>
       </c>
       <c r="G38" s="7">
@@ -63854,8 +64005,12 @@
       <c r="N38" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O38" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>20</v>
       </c>
@@ -63872,7 +64027,7 @@
         <v>494</v>
       </c>
       <c r="F39" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>165.79999999999995</v>
       </c>
       <c r="G39" s="7">
@@ -63899,8 +64054,12 @@
       <c r="N39" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O39" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>22</v>
       </c>
@@ -63917,7 +64076,7 @@
         <v>687</v>
       </c>
       <c r="F40" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="G40" s="7">
@@ -63944,8 +64103,12 @@
       <c r="N40" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O40" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>21</v>
       </c>
@@ -63962,7 +64125,7 @@
         <v>583</v>
       </c>
       <c r="F41" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>123.30000000000001</v>
       </c>
       <c r="G41" s="7">
@@ -63989,8 +64152,12 @@
       <c r="N41" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O41" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>21</v>
       </c>
@@ -64007,7 +64174,7 @@
         <v>469</v>
       </c>
       <c r="F42" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65.800000000000011</v>
       </c>
       <c r="G42" s="7">
@@ -64034,8 +64201,12 @@
       <c r="N42" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O42" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>21</v>
       </c>
@@ -64052,7 +64223,7 @@
         <v>435</v>
       </c>
       <c r="F43" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>118.39999999999998</v>
       </c>
       <c r="G43" s="7">
@@ -64079,8 +64250,12 @@
       <c r="N43" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O43" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>21</v>
       </c>
@@ -64097,7 +64272,7 @@
         <v>196</v>
       </c>
       <c r="F44" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104</v>
       </c>
       <c r="G44" s="7">
@@ -64124,8 +64299,12 @@
       <c r="N44" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O44" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>21</v>
       </c>
@@ -64142,7 +64321,7 @@
         <v>118</v>
       </c>
       <c r="F45" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="G45" s="7">
@@ -64169,8 +64348,12 @@
       <c r="N45" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O45" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>21</v>
       </c>
@@ -64187,7 +64370,7 @@
         <v>109</v>
       </c>
       <c r="F46" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="G46" s="7">
@@ -64214,8 +64397,12 @@
       <c r="N46" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O46" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>21</v>
       </c>
@@ -64232,7 +64419,7 @@
         <v>181</v>
       </c>
       <c r="F47" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>229</v>
       </c>
       <c r="G47" s="7">
@@ -64259,8 +64446,12 @@
       <c r="N47" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O47" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>21</v>
       </c>
@@ -64277,7 +64468,7 @@
         <v>165</v>
       </c>
       <c r="F48" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>222</v>
       </c>
       <c r="G48" s="7">
@@ -64304,8 +64495,12 @@
       <c r="N48" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O48" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>21</v>
       </c>
@@ -64322,7 +64517,7 @@
         <v>19</v>
       </c>
       <c r="F49" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="G49" s="7">
@@ -64349,8 +64544,12 @@
       <c r="N49" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O49" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>21</v>
       </c>
@@ -64367,7 +64566,7 @@
         <v>48</v>
       </c>
       <c r="F50" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>158</v>
       </c>
       <c r="G50" s="7">
@@ -64394,8 +64593,12 @@
       <c r="N50" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O50" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>23</v>
       </c>
@@ -64412,7 +64615,7 @@
         <v>957</v>
       </c>
       <c r="F51" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63.600000000000023</v>
       </c>
       <c r="G51" s="7">
@@ -64439,8 +64642,12 @@
       <c r="N51" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O51" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>23</v>
       </c>
@@ -64457,7 +64664,7 @@
         <v>526</v>
       </c>
       <c r="F52" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>84.199999999999989</v>
       </c>
       <c r="G52" s="7">
@@ -64484,8 +64691,12 @@
       <c r="N52" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O52" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>23</v>
       </c>
@@ -64502,7 +64713,7 @@
         <v>214</v>
       </c>
       <c r="F53" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>78</v>
       </c>
       <c r="G53" s="7">
@@ -64529,8 +64740,12 @@
       <c r="N53" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O53" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>24</v>
       </c>
@@ -64547,7 +64762,7 @@
         <v>889</v>
       </c>
       <c r="F54" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49.899999999999977</v>
       </c>
       <c r="G54" s="7">
@@ -64574,8 +64789,12 @@
       <c r="N54" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O54" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>24</v>
       </c>
@@ -64592,7 +64811,7 @@
         <v>459</v>
       </c>
       <c r="F55" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>67.800000000000011</v>
       </c>
       <c r="G55" s="7">
@@ -64619,8 +64838,12 @@
       <c r="N55" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O55" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>24</v>
       </c>
@@ -64637,7 +64860,7 @@
         <v>237</v>
       </c>
       <c r="F56" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
       <c r="G56" s="7">
@@ -64664,8 +64887,12 @@
       <c r="N56" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O56" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>26</v>
       </c>
@@ -64682,7 +64909,7 @@
         <v>548</v>
       </c>
       <c r="F57" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>203.3</v>
       </c>
       <c r="G57" s="7">
@@ -64709,8 +64936,12 @@
       <c r="N57" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O57" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>27</v>
       </c>
@@ -64754,8 +64985,12 @@
       <c r="N58" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O58" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>28</v>
       </c>
@@ -64772,7 +65007,7 @@
         <v>359</v>
       </c>
       <c r="F59" s="7">
-        <f t="shared" ref="F59:F89" si="2">MOD(180+G59,360)</f>
+        <f t="shared" ref="F59:F89" si="3">MOD(180+G59,360)</f>
         <v>72.5</v>
       </c>
       <c r="G59" s="7">
@@ -64799,8 +65034,12 @@
       <c r="N59" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O59" t="str">
+        <f t="shared" si="1"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>29</v>
       </c>
@@ -64817,7 +65056,7 @@
         <v>619</v>
       </c>
       <c r="F60" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>88.199999999999989</v>
       </c>
       <c r="G60" s="7">
@@ -64844,8 +65083,12 @@
       <c r="N60" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O60" t="str">
+        <f t="shared" si="1"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>30</v>
       </c>
@@ -64862,7 +65105,7 @@
         <v>197</v>
       </c>
       <c r="F61" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="G61" s="7">
@@ -64889,8 +65132,12 @@
       <c r="N61" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O61" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>30</v>
       </c>
@@ -64907,7 +65154,7 @@
         <v>404</v>
       </c>
       <c r="F62" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>293.10000000000002</v>
       </c>
       <c r="G62" s="7">
@@ -64934,8 +65181,12 @@
       <c r="N62" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O62" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>30</v>
       </c>
@@ -64952,7 +65203,7 @@
         <v>503</v>
       </c>
       <c r="F63" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>295.60000000000002</v>
       </c>
       <c r="G63" s="7">
@@ -64979,8 +65230,12 @@
       <c r="N63" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O63" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>30</v>
       </c>
@@ -64997,7 +65252,7 @@
         <v>493</v>
       </c>
       <c r="F64" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>261.2</v>
       </c>
       <c r="G64" s="7">
@@ -65024,8 +65279,12 @@
       <c r="N64" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O64" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>30</v>
       </c>
@@ -65042,7 +65301,7 @@
         <v>939</v>
       </c>
       <c r="F65" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>227.10000000000002</v>
       </c>
       <c r="G65" s="7">
@@ -65069,8 +65328,12 @@
       <c r="N65" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O65" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>30</v>
       </c>
@@ -65087,7 +65350,7 @@
         <v>891</v>
       </c>
       <c r="F66" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>297.2</v>
       </c>
       <c r="G66" s="7">
@@ -65114,8 +65377,12 @@
       <c r="N66" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O66" t="str">
+        <f t="shared" si="1"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>30</v>
       </c>
@@ -65132,7 +65399,7 @@
         <v>504</v>
       </c>
       <c r="F67" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>295.8</v>
       </c>
       <c r="G67" s="7">
@@ -65159,8 +65426,12 @@
       <c r="N67" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O67" t="str">
+        <f t="shared" ref="O67:O89" si="4">IF(N67="Landelijk", "Rural", IF(N67="Randstedelijk", "Suburban", "Urban"))</f>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>31</v>
       </c>
@@ -65177,7 +65448,7 @@
         <v>1058</v>
       </c>
       <c r="F68" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>114.19999999999999</v>
       </c>
       <c r="G68" s="7">
@@ -65204,8 +65475,12 @@
       <c r="N68" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O68" t="str">
+        <f t="shared" si="4"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>31</v>
       </c>
@@ -65222,7 +65497,7 @@
         <v>846</v>
       </c>
       <c r="F69" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>151.80000000000001</v>
       </c>
       <c r="G69" s="7">
@@ -65249,8 +65524,12 @@
       <c r="N69" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O69" t="str">
+        <f t="shared" si="4"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>32</v>
       </c>
@@ -65267,7 +65546,7 @@
         <v>448</v>
       </c>
       <c r="F70" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>48.399999999999977</v>
       </c>
       <c r="G70" s="7">
@@ -65294,8 +65573,12 @@
       <c r="N70" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O70" t="str">
+        <f t="shared" si="4"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>32</v>
       </c>
@@ -65312,7 +65595,7 @@
         <v>241</v>
       </c>
       <c r="F71" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>73</v>
       </c>
       <c r="G71" s="7">
@@ -65339,8 +65622,12 @@
       <c r="N71" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O71" t="str">
+        <f t="shared" si="4"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>33</v>
       </c>
@@ -65357,7 +65644,7 @@
         <v>78</v>
       </c>
       <c r="F72" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>113</v>
       </c>
       <c r="G72" s="7">
@@ -65384,8 +65671,12 @@
       <c r="N72" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O72" t="str">
+        <f t="shared" si="4"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>34</v>
       </c>
@@ -65402,7 +65693,7 @@
         <v>980</v>
       </c>
       <c r="F73" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>252.8</v>
       </c>
       <c r="G73" s="7">
@@ -65429,8 +65720,12 @@
       <c r="N73" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O73" t="str">
+        <f t="shared" si="4"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>34</v>
       </c>
@@ -65447,7 +65742,7 @@
         <v>700</v>
       </c>
       <c r="F74" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>336</v>
       </c>
       <c r="G74" s="7">
@@ -65474,8 +65769,12 @@
       <c r="N74" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O74" t="str">
+        <f t="shared" si="4"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>35</v>
       </c>
@@ -65492,7 +65791,7 @@
         <v>684</v>
       </c>
       <c r="F75" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>204.4</v>
       </c>
       <c r="G75" s="7">
@@ -65519,8 +65818,12 @@
       <c r="N75" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O75" t="str">
+        <f t="shared" si="4"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>35</v>
       </c>
@@ -65537,7 +65840,7 @@
         <v>562</v>
       </c>
       <c r="F76" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>171.10000000000002</v>
       </c>
       <c r="G76" s="7">
@@ -65564,8 +65867,12 @@
       <c r="N76" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O76" t="str">
+        <f t="shared" si="4"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>36</v>
       </c>
@@ -65582,7 +65889,7 @@
         <v>439</v>
       </c>
       <c r="F77" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>163</v>
       </c>
       <c r="G77" s="7">
@@ -65609,8 +65916,12 @@
       <c r="N77" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O77" t="str">
+        <f t="shared" si="4"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>36</v>
       </c>
@@ -65627,7 +65938,7 @@
         <v>412</v>
       </c>
       <c r="F78" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>94.300000000000011</v>
       </c>
       <c r="G78" s="7">
@@ -65654,8 +65965,12 @@
       <c r="N78" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O78" t="str">
+        <f t="shared" si="4"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>37</v>
       </c>
@@ -65672,7 +65987,7 @@
         <v>691</v>
       </c>
       <c r="F79" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>171.60000000000002</v>
       </c>
       <c r="G79" s="7">
@@ -65699,8 +66014,12 @@
       <c r="N79" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O79" t="str">
+        <f t="shared" si="4"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>37</v>
       </c>
@@ -65717,7 +66036,7 @@
         <v>412</v>
       </c>
       <c r="F80" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>178.5</v>
       </c>
       <c r="G80" s="7">
@@ -65744,8 +66063,12 @@
       <c r="N80" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O80" t="str">
+        <f t="shared" si="4"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>38</v>
       </c>
@@ -65762,7 +66085,7 @@
         <v>53</v>
       </c>
       <c r="F81" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G81" s="7">
@@ -65789,8 +66112,12 @@
       <c r="N81" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O81" t="str">
+        <f t="shared" si="4"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>38</v>
       </c>
@@ -65807,7 +66134,7 @@
         <v>130</v>
       </c>
       <c r="F82" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>293</v>
       </c>
       <c r="G82" s="7">
@@ -65834,8 +66161,12 @@
       <c r="N82" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O82" t="str">
+        <f t="shared" si="4"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>39</v>
       </c>
@@ -65852,7 +66183,7 @@
         <v>33</v>
       </c>
       <c r="F83" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="G83" s="7">
@@ -65879,8 +66210,12 @@
       <c r="N83" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O83" t="str">
+        <f t="shared" si="4"/>
+        <v>Urban</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>40</v>
       </c>
@@ -65897,7 +66232,7 @@
         <v>164</v>
       </c>
       <c r="F84" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="G84" s="7">
@@ -65924,8 +66259,12 @@
       <c r="N84" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O84" t="str">
+        <f t="shared" si="4"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>40</v>
       </c>
@@ -65942,7 +66281,7 @@
         <v>82</v>
       </c>
       <c r="F85" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>240</v>
       </c>
       <c r="G85" s="7">
@@ -65969,8 +66308,12 @@
       <c r="N85" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O85" t="str">
+        <f t="shared" si="4"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>40</v>
       </c>
@@ -65987,7 +66330,7 @@
         <v>207</v>
       </c>
       <c r="F86" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>280</v>
       </c>
       <c r="G86" s="7">
@@ -66014,8 +66357,12 @@
       <c r="N86" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O86" t="str">
+        <f t="shared" si="4"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>40</v>
       </c>
@@ -66032,7 +66379,7 @@
         <v>248</v>
       </c>
       <c r="F87" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="G87" s="7">
@@ -66059,8 +66406,12 @@
       <c r="N87" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O87" t="str">
+        <f t="shared" si="4"/>
+        <v>Suburban</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>41</v>
       </c>
@@ -66077,7 +66428,7 @@
         <v>869</v>
       </c>
       <c r="F88" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.300000000000011</v>
       </c>
       <c r="G88" s="7">
@@ -66104,8 +66455,12 @@
       <c r="N88" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O88" t="str">
+        <f t="shared" si="4"/>
+        <v>Rural</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>41</v>
       </c>
@@ -66122,7 +66477,7 @@
         <v>1269</v>
       </c>
       <c r="F89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>202</v>
       </c>
       <c r="G89">
@@ -66148,6 +66503,10 @@
       </c>
       <c r="N89" t="s">
         <v>258</v>
+      </c>
+      <c r="O89" t="str">
+        <f t="shared" si="4"/>
+        <v>Rural</v>
       </c>
     </row>
   </sheetData>

</xml_diff>